<commit_message>
Completed and compiled hatespeech
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/other_dr_techniques/K-PCA/m1_results_K-PCA.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/other_dr_techniques/K-PCA/m1_results_K-PCA.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -943,6 +943,98 @@
         <v>0.9999936563670762</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-10-08 10:42:41</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.9932370474835958</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-10-08 10:42:41</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>20</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.9901418096316194</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-10-08 10:42:41</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>30</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9882337531908792</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2023-10-08 10:42:41</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>40</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9867270015936512</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>